<commit_message>
Adaptar el model de PartidasModel.cs para los cambios que sufrieron los campos  PA_STATUS_PARTIDA PA_TIPO_CONCILIA PA_ESTADO_CONCILIA PA_ORIGEN_REFERENCIA
</commit_message>
<xml_diff>
--- a/Banistmo.Sax.WebApi/App_Data/Carga_Prueba_Empresa006.xlsx
+++ b/Banistmo.Sax.WebApi/App_Data/Carga_Prueba_Empresa006.xlsx
@@ -667,9 +667,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI119"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13:BI119"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>